<commit_message>
befotre uploading to hosting
</commit_message>
<xml_diff>
--- a/texts/site.xlsx
+++ b/texts/site.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="60">
   <si>
     <t>Створення сайтів</t>
   </si>
@@ -200,6 +200,12 @@
   </si>
   <si>
     <t>Збереження даних. Ми працюємо над цією сторінкою -   IT майстерня “Все працює”</t>
+  </si>
+  <si>
+    <t>webdesign.html</t>
+  </si>
+  <si>
+    <t>Створення сайтів. Ми працюємо над цією сторінкою -   IT майстерня “Все працює”</t>
   </si>
 </sst>
 </file>
@@ -669,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:B15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -885,82 +891,91 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>21</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
title + description after audit
</commit_message>
<xml_diff>
--- a/texts/site.xlsx
+++ b/texts/site.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11460" activeTab="3"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11460" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="77">
   <si>
     <t>Створення сайтів</t>
   </si>
@@ -179,15 +179,9 @@
     <t>proektuvannya.html</t>
   </si>
   <si>
-    <t>Проектування інфраструктури. Ми працюємо над цією сторінкою -   IT майстерня “Все працює”</t>
-  </si>
-  <si>
     <t>servers.html</t>
   </si>
   <si>
-    <t>Серверна інфраструктура. Ми працюємо над цією сторінкою -   IT майстерня “Все працює”</t>
-  </si>
-  <si>
     <t>videosposteregennya.html</t>
   </si>
   <si>
@@ -213,6 +207,57 @@
   </si>
   <si>
     <t>Патч-корд</t>
+  </si>
+  <si>
+    <t>&lt;meta name="description" content="&amp;#128736; Відеоспостереження.  Сторінка створюється.&amp;#10057;   "&gt;</t>
+  </si>
+  <si>
+    <t>&lt;meta name="description" content="&amp;#128736; Серверна інфраструктура. Сторінка створюється.&amp;#10057;   "&gt;</t>
+  </si>
+  <si>
+    <t>&lt;meta name="description" content="&amp;#128736;Організація локальної мережі.   Сторінка створюється.&amp;#10057;"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;meta name="description" content="&amp;#128736;Збереження дагих. Сторінка створюється.&amp;#10057;"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;meta name="description" content="&amp;#128736;Проектування інфраструктури.  Сторінка створюється.&amp;#10057;"&gt;</t>
+  </si>
+  <si>
+    <t>Проектування інфраструктури. Сторінка створюється - IT майстерня “Все працює”</t>
+  </si>
+  <si>
+    <t>Серверна інфраструктура. Сторінка створюється  -  IT майстерня “Все працює”</t>
+  </si>
+  <si>
+    <t>about.html</t>
+  </si>
+  <si>
+    <t>Про нас - IT майстерня “Все працює”</t>
+  </si>
+  <si>
+    <t>&lt;meta name="description" content="&amp;#128736;Про нас.&amp;#10057;  IT-аутсорсинг для малого бізнесу.&amp;#10057; Абонентське обслуговування від 1000,00 грн. на місяць!&amp;#10057;"&gt;</t>
+  </si>
+  <si>
+    <t>contacts.html</t>
+  </si>
+  <si>
+    <t>Контактна інформація - IT майстерня “Все працює”</t>
+  </si>
+  <si>
+    <t>&lt;meta name="description" content="&amp;#128736;Про нас.&amp;#10057;  Телефонуйте.&amp;#10057; Пишіть.&amp;#10057;"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;meta name="description" content="&amp;#128736;IP-телефонія.  Сторінка створюється.&amp;#10057;"&gt;</t>
+  </si>
+  <si>
+    <t>service-centr.html</t>
+  </si>
+  <si>
+    <t>Сервісний центр - IT майстерня “Все працює”</t>
+  </si>
+  <si>
+    <t>&lt;meta name="description" content="&amp;#128736;Сервісний центр. &amp;#10057; Сторінка створюється.&amp;#10057;   "&gt;</t>
   </si>
 </sst>
 </file>
@@ -690,10 +735,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D56"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,7 +822,7 @@
         <v>41</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -805,315 +850,344 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
         <v>3</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>11</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
+        <v>15</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
         <v>16</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
+      <c r="B16" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
         <v>17</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
+      <c r="B17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
         <v>18</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>19</v>
+      <c r="B18" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
+    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
         <v>21</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D20" s="1" t="s">
+      <c r="B21" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
         <v>57</v>
       </c>
     </row>
@@ -1127,7 +1201,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E10:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -1138,7 +1212,7 @@
   <sheetData>
     <row r="10" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F10">
         <v>240</v>
@@ -1153,7 +1227,7 @@
     </row>
     <row r="11" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F11">
         <v>60</v>

</xml_diff>

<commit_message>
titles + descriptions at home
</commit_message>
<xml_diff>
--- a/texts/site.xlsx
+++ b/texts/site.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11460" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11460" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="85">
   <si>
     <t>Створення сайтів</t>
   </si>
@@ -116,15 +116,6 @@
     <t>Обслуговування комп'ютерів, мереж, серверів  в Києві- IT майстерня “Все працює”</t>
   </si>
   <si>
-    <t>&lt;meta name="description" content="&amp;#128736; Буде інтернет. &amp;#10057; Файли будуть відкриватись.  &amp;#10057; Документи будуть друкуватись. &amp;#10057;   Заходьте, порозуміємось!"&gt;</t>
-  </si>
-  <si>
-    <t>&lt;meta name="description" content="&amp;#128736;IT аутсорсінг для малого бізнесу. &amp;#10057; Навіть якщо ваша інфраструктура складається з одного комп'ютера, ми готові працювати для вас. &amp;#10057; Заходьте, порозуміємось!"&gt;</t>
-  </si>
-  <si>
-    <t>&lt;meta name="description" content="&amp;#128736; Обмеження за кількістю виїздів відсутні.&amp;#10057; Реагуємо за 15 хвилин. &amp;#10057; Від 1000,00 грн.&amp;#10057;  На сайті є калькулятор вартості.  Заходьте, порозуміємось!"&gt;</t>
-  </si>
-  <si>
     <t>&lt;meta name="description" content="&amp;#128736;Створимо з нуля, або модернізуємо те, що є.&amp;#10057; Ваша інфраструктура буде працювати на вас. &amp;#10057; Сьогодні та в майбутньому.&amp;#10057; Заходьте, порозуміємось!"&gt;</t>
   </si>
   <si>
@@ -273,6 +264,24 @@
   </si>
   <si>
     <t>&lt;meta name="description" content="&amp;#128736; Ограничения  количества виездов отсутствуют.&amp;#10057; Реагируем за 15 минут. &amp;#10057; От 1000,00 грн.&amp;#10057;  На сайте есть калькулятор стоимости.  Заходите, договоримся!"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;meta name="description" content="&amp;#128736;Ми вміємо створювати та обслуговувати інформаційну інфраструктуру. &amp;#10057;Ми пропонуємо IT-аутсорсінг для малого бізнесу. &amp;#10057;Навіть якщо ваша інфраструктура складається з одного комп'ютера, ми готові працювати для вас. &amp;#10057; Заходьте, порозуміємось!"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;meta name="description" content="&amp;#128736; В вас завжди буде інтернет. &amp;#10057; Файли будуть знаходитись там, де треба й завжди будуть відкриватись.  &amp;#10057; Документи будуть друкуватись. &amp;#10057; IP-телефонія заощадить час вашіх працівників. &amp;#10057;Заходьте, порозуміємось!"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;meta name="description" content="&amp;#128736; Абонентське обслуговування інформаційної інфраструктури.&amp;#10057;Обмеження за кількістю виїздів відсутні.&amp;#10057; Реагуємо за 15 хвилин. &amp;#10057; Від 1000,00 грн.&amp;#10057;  На сайті є калькулятор вартості. &amp;#10057;  Заходьте, порозуміємось!"&gt;</t>
+  </si>
+  <si>
+    <t>Вартість абонентського обслуговування - IT майстерня “Все працює”.</t>
+  </si>
+  <si>
+    <t>&lt;meta name="description" content="&amp;#128736; Скільки коштує абонентське обслуговування?&amp;#10057; Що за ці гроші отримує клієнт?&amp;#10057;Калькулятор вартості. &amp;#10057; Заходьте, порозуміємось!"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;meta name="description" content="&amp;#128736;Вирішимо будь-яку IT проблему. &amp;#10057; Ви завжди будете знать скільки й за що ви платите.  &amp;#10057; Рекомендації безкоштовні.&amp;#10057; Реагуємо протягом 15 хвилин.&amp;#10057;    Заходьте, порозуміємось!"&gt;</t>
   </si>
 </sst>
 </file>
@@ -289,7 +298,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -308,6 +317,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -321,7 +336,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -330,6 +345,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -742,8 +760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A4" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -766,7 +784,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -774,13 +792,13 @@
         <v>22</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -791,10 +809,10 @@
         <v>28</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>4</v>
       </c>
@@ -802,43 +820,43 @@
         <v>25</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>36</v>
+        <v>82</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -849,21 +867,21 @@
         <v>26</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>33</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -874,10 +892,10 @@
         <v>24</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -885,13 +903,13 @@
         <v>11</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -899,13 +917,13 @@
         <v>12</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -913,13 +931,13 @@
         <v>13</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -927,13 +945,13 @@
         <v>14</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -941,13 +959,13 @@
         <v>15</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -955,13 +973,13 @@
         <v>16</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -969,13 +987,13 @@
         <v>17</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -983,13 +1001,13 @@
         <v>18</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1007,13 +1025,13 @@
         <v>21</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1206,7 +1224,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -1238,10 +1256,10 @@
         <v>22</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1252,10 +1270,10 @@
         <v>23</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1266,10 +1284,10 @@
         <v>25</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1277,32 +1295,32 @@
         <v>27</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1313,21 +1331,21 @@
         <v>26</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1338,10 +1356,10 @@
         <v>24</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1349,13 +1367,13 @@
         <v>11</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1363,13 +1381,13 @@
         <v>12</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1377,13 +1395,13 @@
         <v>13</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1391,13 +1409,13 @@
         <v>14</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1405,13 +1423,13 @@
         <v>15</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1419,13 +1437,13 @@
         <v>16</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1433,13 +1451,13 @@
         <v>17</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1447,13 +1465,13 @@
         <v>18</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1471,13 +1489,13 @@
         <v>21</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>